<commit_message>
Running some evaluations. #macosbytecode
</commit_message>
<xml_diff>
--- a/linuxRunners/some results.xlsx
+++ b/linuxRunners/some results.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="480" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="2580" yWindow="480" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="01data" sheetId="2" r:id="rId1"/>
-    <sheet name="02data" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
+    <sheet name="01data-ok" sheetId="2" r:id="rId1"/>
+    <sheet name="02data-ok" sheetId="3" r:id="rId2"/>
+    <sheet name="03data-ok" sheetId="5" r:id="rId3"/>
+    <sheet name="04data-ok" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="28">
   <si>
     <t>LOOPS=40</t>
   </si>
@@ -62,84 +63,60 @@
     <t>defautla node size = 10</t>
   </si>
   <si>
-    <t xml:space="preserve">ROUNDS=1000000 </t>
+    <t xml:space="preserve">		&lt;dimX value="3000" /&gt;</t>
   </si>
   <si>
-    <t>REFRESHRATE=1000000</t>
+    <t xml:space="preserve">		&lt;dimY value="1250" /&gt;</t>
   </si>
   <si>
-    <t>28 para 29/0/2016</t>
+    <t>31/07/2016</t>
   </si>
   <si>
-    <t>LOOPS=5</t>
+    <t>LOOPS=3</t>
   </si>
   <si>
-    <t xml:space="preserve">		&lt;dimX value="6000" /&gt;</t>
+    <t>nUAV:  2 4 8 16</t>
   </si>
   <si>
-    <t xml:space="preserve">		&lt;dimY value="2500" /&gt;</t>
+    <t>POIs:  20</t>
   </si>
   <si>
-    <t xml:space="preserve"> counter = 12</t>
+    <t>X * Y ?</t>
   </si>
   <si>
-    <t>.48271833333333333333</t>
+    <t>ROUNDS=3750000</t>
   </si>
   <si>
-    <t>.69680833333333333333</t>
+    <t>REFRESHRATE=1</t>
   </si>
   <si>
-    <t>.01096083333333333333</t>
+    <t>LOOPS=10</t>
   </si>
   <si>
-    <t>.01975166666666666666</t>
+    <t>NotSoNaiveOrderedMobility</t>
   </si>
   <si>
-    <t>.04055000000000000000</t>
+    <t>TSPbased - NP-hard</t>
   </si>
   <si>
-    <t>.05369500000000000000</t>
+    <t>NotSoNaiveOrdered O(n2)</t>
   </si>
   <si>
-    <t>.35188166666666666666</t>
+    <t>NaiveOrdered     O(n log n)</t>
   </si>
   <si>
-    <t>.69531500000000000000</t>
-  </si>
-  <si>
-    <t>.41320000000000000000</t>
-  </si>
-  <si>
-    <t>.86178916666666666666</t>
-  </si>
-  <si>
-    <t>KingstonImprovedMobility; counter = 12
-KingstonImprovedMobility;1;.48271833333333333333
-KingstonImprovedMobility;2;.69680833333333333333
-KingstonImprovedMobility;4;1.70547166666666666666
-KingstonImprovedMobility;6;2.52105666666666666666
-RandomSafeMobility; counter = 12
-RandomSafeMobility;1;.01096083333333333333
-RandomSafeMobility;2;.01975166666666666666
-RandomSafeMobility;4;.04055000000000000000
-RandomSafeMobility;6;.05369500000000000000
-NaiveOrderedMobility; counter = 12
-NaiveOrderedMobility;1;.35188166666666666666
-NaiveOrderedMobility;2;.69531500000000000000
-NaiveOrderedMobility;4;1.42302750000000000000
-NaiveOrderedMobility;6;2.18513333333333333333
-TSPbasedMobility; counter = 12
-TSPbasedMobility;1;.41320000000000000000
-TSPbasedMobility;2;.86178916666666666666
-TSPbasedMobility;4;1.67788416666666666666
-TSPbasedMobility;6;2.94074833333333333333</t>
+    <t>KingstonImproved (Distribuído)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -163,6 +140,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -181,7 +165,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -191,23 +175,64 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -240,7 +265,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01data'!$A$1</c:f>
+              <c:f>'01data-ok'!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -254,7 +279,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'01data'!$B$17:$B$20</c:f>
+              <c:f>'01data-ok'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -275,7 +300,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'01data'!$C$1:$C$4</c:f>
+              <c:f>'01data-ok'!$C$1:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -301,7 +326,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01data'!$A$7</c:f>
+              <c:f>'01data-ok'!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -315,7 +340,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'01data'!$B$17:$B$20</c:f>
+              <c:f>'01data-ok'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -336,7 +361,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'01data'!$C$5:$C$8</c:f>
+              <c:f>'01data-ok'!$C$5:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -362,7 +387,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01data'!$A$10</c:f>
+              <c:f>'01data-ok'!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -376,7 +401,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'01data'!$B$17:$B$20</c:f>
+              <c:f>'01data-ok'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -397,7 +422,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'01data'!$C$9:$C$12</c:f>
+              <c:f>'01data-ok'!$C$9:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -423,7 +448,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01data'!$A$14</c:f>
+              <c:f>'01data-ok'!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -437,7 +462,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'01data'!$B$17:$B$20</c:f>
+              <c:f>'01data-ok'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -458,7 +483,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'01data'!$C$13:$C$16</c:f>
+              <c:f>'01data-ok'!$C$13:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -484,7 +509,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01data'!$A$18</c:f>
+              <c:f>'01data-ok'!$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -498,7 +523,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'01data'!$B$17:$B$20</c:f>
+              <c:f>'01data-ok'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -519,7 +544,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'01data'!$C$17:$C$20</c:f>
+              <c:f>'01data-ok'!$C$17:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -550,11 +575,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2132354744"/>
-        <c:axId val="-2132399112"/>
+        <c:axId val="2079457864"/>
+        <c:axId val="2079454792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2132354744"/>
+        <c:axId val="2079457864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -564,7 +589,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132399112"/>
+        <c:crossAx val="2079454792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -572,7 +597,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2132399112"/>
+        <c:axId val="2079454792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -583,7 +608,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132354744"/>
+        <c:crossAx val="2079457864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -630,7 +655,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01data'!$A$1</c:f>
+              <c:f>'01data-ok'!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -644,7 +669,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'01data'!$B$17:$B$20</c:f>
+              <c:f>'01data-ok'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -665,7 +690,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'01data'!$C$1:$C$4</c:f>
+              <c:f>'01data-ok'!$C$1:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -691,7 +716,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01data'!$A$10</c:f>
+              <c:f>'01data-ok'!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -705,7 +730,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'01data'!$B$17:$B$20</c:f>
+              <c:f>'01data-ok'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -726,7 +751,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'01data'!$C$9:$C$12</c:f>
+              <c:f>'01data-ok'!$C$9:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -752,7 +777,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01data'!$A$14</c:f>
+              <c:f>'01data-ok'!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -766,7 +791,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'01data'!$B$17:$B$20</c:f>
+              <c:f>'01data-ok'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -787,7 +812,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'01data'!$C$13:$C$16</c:f>
+              <c:f>'01data-ok'!$C$13:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -818,11 +843,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2132692280"/>
-        <c:axId val="-2132689224"/>
+        <c:axId val="2124790648"/>
+        <c:axId val="2124793624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2132692280"/>
+        <c:axId val="2124790648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -832,7 +857,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132689224"/>
+        <c:crossAx val="2124793624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -840,7 +865,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2132689224"/>
+        <c:axId val="2124793624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -851,7 +876,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132692280"/>
+        <c:crossAx val="2124790648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -898,7 +923,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02data'!$A$1</c:f>
+              <c:f>'02data-ok'!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -912,7 +937,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'02data'!$B$17:$B$20</c:f>
+              <c:f>'02data-ok'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -921,10 +946,22 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'02data'!$C$1:$C$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+              <c:f>'02data-ok'!$C$1:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.12964</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.26967333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.49184666666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.6112833333333</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -935,11 +972,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02data'!$A$7</c:f>
+              <c:f>'02data-ok'!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>RandomSafeMobility</c:v>
+                  <c:v>NaiveOrderedMobility</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -949,7 +986,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'02data'!$B$17:$B$20</c:f>
+              <c:f>'02data-ok'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -958,10 +995,22 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'02data'!$C$5:$C$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+              <c:f>'02data-ok'!$C$5:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.41986333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.70500666666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.3276666666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.9068066666666</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -972,11 +1021,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02data'!$A$10</c:f>
+              <c:f>'02data-ok'!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>NaiveOrderedMobility</c:v>
+                  <c:v>TSPbasedMobility</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -986,7 +1035,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'02data'!$B$17:$B$20</c:f>
+              <c:f>'02data-ok'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -995,10 +1044,22 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'02data'!$C$9:$C$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+              <c:f>'02data-ok'!$C$9:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.73517666666666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.21281666666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.4315366666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.9123366666666</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1009,12 +1070,9 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02data'!$A$14</c:f>
+              <c:f>'02data-ok'!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>TSPbasedMobility</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -1023,7 +1081,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'02data'!$B$17:$B$20</c:f>
+              <c:f>'02data-ok'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1032,7 +1090,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'02data'!$C$13:$C$16</c:f>
+              <c:f>'02data-ok'!$C$13:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1046,12 +1104,9 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02data'!$A$18</c:f>
+              <c:f>'02data-ok'!$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>AntiTSPbasedMobility</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -1060,7 +1115,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'02data'!$B$17:$B$20</c:f>
+              <c:f>'02data-ok'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1069,7 +1124,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'02data'!$C$17:$C$20</c:f>
+              <c:f>'02data-ok'!$C$17:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1088,11 +1143,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2125139400"/>
-        <c:axId val="-2125136344"/>
+        <c:axId val="2126766488"/>
+        <c:axId val="2126769544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2125139400"/>
+        <c:axId val="2126766488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1102,7 +1157,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2125136344"/>
+        <c:crossAx val="2126769544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1110,7 +1165,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2125136344"/>
+        <c:axId val="2126769544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1121,7 +1176,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2125139400"/>
+        <c:crossAx val="2126766488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1168,7 +1223,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02data'!$A$1</c:f>
+              <c:f>'02data-ok'!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1182,19 +1237,43 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'02data'!$B$17:$B$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+              <c:f>'02data-ok'!$B$5:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'02data'!$C$1:$C$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+              <c:f>'02data-ok'!$C$1:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.12964</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.26967333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.49184666666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.6112833333333</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1205,11 +1284,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02data'!$A$10</c:f>
+              <c:f>'02data-ok'!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>NaiveOrderedMobility</c:v>
+                  <c:v>TSPbasedMobility</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1219,19 +1298,43 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'02data'!$B$17:$B$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+              <c:f>'02data-ok'!$B$5:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'02data'!$C$9:$C$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+              <c:f>'02data-ok'!$C$9:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.73517666666666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.21281666666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.4315366666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.9123366666666</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1242,11 +1345,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02data'!$A$14</c:f>
+              <c:f>'02data-ok'!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TSPbasedMobility</c:v>
+                  <c:v>NaiveOrderedMobility</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1256,19 +1359,43 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'02data'!$B$17:$B$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+              <c:f>'02data-ok'!$B$5:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'02data'!$C$13:$C$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+              <c:f>'02data-ok'!$C$5:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.41986333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.70500666666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.3276666666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.9068066666666</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1284,11 +1411,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2126191928"/>
-        <c:axId val="-2129938600"/>
+        <c:axId val="2126800664"/>
+        <c:axId val="2126803640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2126191928"/>
+        <c:axId val="2126800664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1298,7 +1425,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129938600"/>
+        <c:crossAx val="2126803640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1306,7 +1433,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129938600"/>
+        <c:axId val="2126803640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1317,7 +1444,604 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126191928"/>
+        <c:crossAx val="2126800664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'03data-ok'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KingstonImprovedMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'03data-ok'!$B$5:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'03data-ok'!$C$1:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.326367</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.415144</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.568044</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.23651</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'03data-ok'!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TSPbasedMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'03data-ok'!$B$5:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'03data-ok'!$C$9:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.558494</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.218551</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.108468</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.444289</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'03data-ok'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NotSoNaiveOrderedMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'03data-ok'!$B$5:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'03data-ok'!$C$5:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.131371</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.47067</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.624524</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.825341</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2140388328"/>
+        <c:axId val="2140955848"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2140388328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2140955848"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2140955848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#.##00000" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2140388328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'04data-ok'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KingstonImproved (Distribuído)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'04data-ok'!$B$13:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'04data-ok'!$C$1:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.15042829268292</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.83115121951219</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.3326565853658</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.3928780487804</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'04data-ok'!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TSPbased - NP-hard</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'04data-ok'!$B$13:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'04data-ok'!$C$9:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.615052</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.897811</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.823088</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.028619</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'04data-ok'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NotSoNaiveOrdered O(n2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'04data-ok'!$B$13:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'04data-ok'!$C$5:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.183175</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.293619</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.641666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.613135</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'04data-ok'!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NaiveOrdered     O(n log n)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'04data-ok'!$B$13:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'04data-ok'!$C$13:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.247444</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.693923</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.535141</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.742145</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2126418408"/>
+        <c:axId val="-2126272568"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2126418408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2126272568"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2126272568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#.##00000" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2126418408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1467,6 +2191,80 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2079,10 +2877,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A33"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2092,144 +2890,189 @@
     <col min="3" max="3" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3.1296400000000002</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>6.2696733333333299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>8.4918466666666603</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="B4">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>24.611283333333301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>3.4198633333333301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>6.7050066666666597</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>14.3276666666666</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>25.906806666666601</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>3.7351766666666602</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>7.2128166666666598</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>13.431536666666601</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B12">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>27.912336666666601</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
+        <v>20</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2246,233 +3089,464 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C9:E30"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="42.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="4.83203125" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="3:5">
-      <c r="C9" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="D9" t="s">
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4">
+        <v>3.3263669999999999</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4">
+        <v>6.4151439999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4">
+        <v>12.568044</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4">
+        <v>28.236509999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3.1313710000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4">
+        <v>6.4706700000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7" s="4">
+        <v>12.624523999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>16</v>
+      </c>
+      <c r="C8" s="4">
+        <v>23.825341000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4">
+        <v>3.558494</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" s="4">
+        <v>7.2185509999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4">
+        <v>14.108468</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>16</v>
+      </c>
+      <c r="C12" s="4">
+        <v>29.444289000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="3:5">
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="3:5">
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11" t="s">
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="3:5">
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12">
-        <v>4</v>
-      </c>
-      <c r="E12" s="1">
-        <v>1.7054716666666598E+20</v>
-      </c>
-    </row>
-    <row r="13" spans="3:5">
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13">
-        <v>6</v>
-      </c>
-      <c r="E13" s="1">
-        <v>2.52105666666666E+20</v>
-      </c>
-    </row>
-    <row r="14" spans="3:5">
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="3:5">
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="3:5">
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-      <c r="E16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5">
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17">
-        <v>4</v>
-      </c>
-      <c r="E17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5">
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18">
-        <v>6</v>
-      </c>
-      <c r="E18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="3:5">
-      <c r="C19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5">
-      <c r="C20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="3:5">
-      <c r="C21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21">
-        <v>2</v>
-      </c>
-      <c r="E21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="3:5">
-      <c r="C22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22">
-        <v>4</v>
-      </c>
-      <c r="E22" s="1">
-        <v>1.4230275000000001E+20</v>
-      </c>
-    </row>
-    <row r="23" spans="3:5">
-      <c r="C23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23">
-        <v>6</v>
-      </c>
-      <c r="E23" s="1">
-        <v>2.1851333333333298E+20</v>
-      </c>
-    </row>
-    <row r="24" spans="3:5">
-      <c r="C24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="3:5">
-      <c r="C25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="3:5">
-      <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26">
-        <v>2</v>
-      </c>
-      <c r="E26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="3:5">
-      <c r="C27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27">
-        <v>4</v>
-      </c>
-      <c r="E27" s="1">
-        <v>1.6778841666666601E+20</v>
-      </c>
-    </row>
-    <row r="28" spans="3:5">
-      <c r="C28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28">
-        <v>6</v>
-      </c>
-      <c r="E28" s="1">
-        <v>2.94074833333333E+20</v>
-      </c>
-    </row>
-    <row r="30" spans="3:5" ht="390">
-      <c r="C30" s="2" t="s">
-        <v>30</v>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="4.83203125" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4">
+        <v>3.1504282926829199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4">
+        <v>6.83115121951219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4">
+        <v>12.3326565853658</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4">
+        <v>26.3928780487804</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3.1831749999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4">
+        <v>6.2936189999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7" s="4">
+        <v>12.641666000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>16</v>
+      </c>
+      <c r="C8" s="4">
+        <v>25.613135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4">
+        <v>3.6150519999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" s="4">
+        <v>6.8978109999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4">
+        <v>13.823088</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12">
+        <v>16</v>
+      </c>
+      <c r="C12" s="4">
+        <v>28.028618999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1.247444</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2.6939229999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15" s="4">
+        <v>5.5351410000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16">
+        <v>16</v>
+      </c>
+      <c r="C16" s="4">
+        <v>10.742145000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Refactoring kingstonimproved basics to ZigZag Strategy, over two previous naive. Now we have working: Ramdom TSP (max & min) Naive nlogn Naive nˆ2 ZigZag over Naive nlogn ZigZag over Naive nˆ2
#macbytecodes
</commit_message>
<xml_diff>
--- a/linuxRunners/some results.xlsx
+++ b/linuxRunners/some results.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="2580" yWindow="480" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="01data-ok" sheetId="2" r:id="rId1"/>
-    <sheet name="02data-ok" sheetId="3" r:id="rId2"/>
-    <sheet name="03data-ok" sheetId="5" r:id="rId3"/>
-    <sheet name="04data-ok" sheetId="6" r:id="rId4"/>
+    <sheet name="01data-Alpha" sheetId="2" r:id="rId1"/>
+    <sheet name="02data-bad" sheetId="3" r:id="rId2"/>
+    <sheet name="03data-beta" sheetId="5" r:id="rId3"/>
+    <sheet name="04data-beta" sheetId="6" r:id="rId4"/>
     <sheet name="05data-running" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="34">
   <si>
     <t>LOOPS=40</t>
   </si>
@@ -109,19 +109,22 @@
     <t>KingstonImproved (Distribuído) + NotSoNaive</t>
   </si>
   <si>
-    <t>NotSoNaive + KingstonImproved (Distribuído)</t>
-  </si>
-  <si>
-    <t>Naive + KingstonImproved</t>
-  </si>
-  <si>
     <t>LOOPS=30</t>
   </si>
   <si>
-    <t>POIs:  15</t>
+    <t>ZigZagOverNSNMobility</t>
   </si>
   <si>
-    <t>nUAV:  2 4 6 8</t>
+    <t>ZigZagOverNaiveMobility</t>
+  </si>
+  <si>
+    <t>POIs:  30</t>
+  </si>
+  <si>
+    <t>30 é o minimo do minimo</t>
+  </si>
+  <si>
+    <t>Hard to run on TSP</t>
   </si>
 </sst>
 </file>
@@ -130,7 +133,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -181,7 +184,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -233,16 +236,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -268,6 +277,8 @@
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -293,6 +304,8 @@
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -325,7 +338,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01data-ok'!$A$1</c:f>
+              <c:f>'01data-Alpha'!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -339,7 +352,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'01data-ok'!$B$17:$B$20</c:f>
+              <c:f>'01data-Alpha'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -360,7 +373,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'01data-ok'!$C$1:$C$4</c:f>
+              <c:f>'01data-Alpha'!$C$1:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -386,7 +399,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01data-ok'!$A$7</c:f>
+              <c:f>'01data-Alpha'!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -400,7 +413,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'01data-ok'!$B$17:$B$20</c:f>
+              <c:f>'01data-Alpha'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -421,7 +434,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'01data-ok'!$C$5:$C$8</c:f>
+              <c:f>'01data-Alpha'!$C$5:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -447,7 +460,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01data-ok'!$A$10</c:f>
+              <c:f>'01data-Alpha'!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -461,7 +474,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'01data-ok'!$B$17:$B$20</c:f>
+              <c:f>'01data-Alpha'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -482,7 +495,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'01data-ok'!$C$9:$C$12</c:f>
+              <c:f>'01data-Alpha'!$C$9:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -508,7 +521,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01data-ok'!$A$14</c:f>
+              <c:f>'01data-Alpha'!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -522,7 +535,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'01data-ok'!$B$17:$B$20</c:f>
+              <c:f>'01data-Alpha'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -543,7 +556,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'01data-ok'!$C$13:$C$16</c:f>
+              <c:f>'01data-Alpha'!$C$13:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -569,7 +582,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01data-ok'!$A$18</c:f>
+              <c:f>'01data-Alpha'!$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -583,7 +596,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'01data-ok'!$B$17:$B$20</c:f>
+              <c:f>'01data-Alpha'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -604,7 +617,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'01data-ok'!$C$17:$C$20</c:f>
+              <c:f>'01data-Alpha'!$C$17:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -635,11 +648,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2079457864"/>
-        <c:axId val="2079454792"/>
+        <c:axId val="2081307112"/>
+        <c:axId val="2081310168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2079457864"/>
+        <c:axId val="2081307112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -649,7 +662,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079454792"/>
+        <c:crossAx val="2081310168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -657,7 +670,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2079454792"/>
+        <c:axId val="2081310168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -668,7 +681,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079457864"/>
+        <c:crossAx val="2081307112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -715,7 +728,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01data-ok'!$A$1</c:f>
+              <c:f>'01data-Alpha'!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -729,7 +742,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'01data-ok'!$B$17:$B$20</c:f>
+              <c:f>'01data-Alpha'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -750,7 +763,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'01data-ok'!$C$1:$C$4</c:f>
+              <c:f>'01data-Alpha'!$C$1:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -776,7 +789,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01data-ok'!$A$10</c:f>
+              <c:f>'01data-Alpha'!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -790,7 +803,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'01data-ok'!$B$17:$B$20</c:f>
+              <c:f>'01data-Alpha'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -811,7 +824,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'01data-ok'!$C$9:$C$12</c:f>
+              <c:f>'01data-Alpha'!$C$9:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -837,7 +850,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01data-ok'!$A$14</c:f>
+              <c:f>'01data-Alpha'!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -851,7 +864,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'01data-ok'!$B$17:$B$20</c:f>
+              <c:f>'01data-Alpha'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -872,7 +885,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'01data-ok'!$C$13:$C$16</c:f>
+              <c:f>'01data-Alpha'!$C$13:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -903,11 +916,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2124790648"/>
-        <c:axId val="2124793624"/>
+        <c:axId val="2081340200"/>
+        <c:axId val="2081343176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2124790648"/>
+        <c:axId val="2081340200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -917,7 +930,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124793624"/>
+        <c:crossAx val="2081343176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -925,7 +938,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2124793624"/>
+        <c:axId val="2081343176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -936,7 +949,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124790648"/>
+        <c:crossAx val="2081340200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -983,7 +996,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02data-ok'!$A$1</c:f>
+              <c:f>'02data-bad'!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -997,7 +1010,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'02data-ok'!$B$17:$B$20</c:f>
+              <c:f>'02data-bad'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1006,7 +1019,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'02data-ok'!$C$1:$C$4</c:f>
+              <c:f>'02data-bad'!$C$1:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1032,7 +1045,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02data-ok'!$A$7</c:f>
+              <c:f>'02data-bad'!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1046,7 +1059,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'02data-ok'!$B$17:$B$20</c:f>
+              <c:f>'02data-bad'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1055,7 +1068,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'02data-ok'!$C$5:$C$8</c:f>
+              <c:f>'02data-bad'!$C$5:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1081,7 +1094,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02data-ok'!$A$10</c:f>
+              <c:f>'02data-bad'!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1095,7 +1108,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'02data-ok'!$B$17:$B$20</c:f>
+              <c:f>'02data-bad'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1104,7 +1117,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'02data-ok'!$C$9:$C$12</c:f>
+              <c:f>'02data-bad'!$C$9:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1130,7 +1143,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02data-ok'!$A$14</c:f>
+              <c:f>'02data-bad'!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -1141,7 +1154,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'02data-ok'!$B$17:$B$20</c:f>
+              <c:f>'02data-bad'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1150,7 +1163,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'02data-ok'!$C$13:$C$16</c:f>
+              <c:f>'02data-bad'!$C$13:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1164,7 +1177,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02data-ok'!$A$18</c:f>
+              <c:f>'02data-bad'!$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -1175,7 +1188,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'02data-ok'!$B$17:$B$20</c:f>
+              <c:f>'02data-bad'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1184,7 +1197,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'02data-ok'!$C$17:$C$20</c:f>
+              <c:f>'02data-bad'!$C$17:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1203,11 +1216,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2126766488"/>
-        <c:axId val="2126769544"/>
+        <c:axId val="2081390728"/>
+        <c:axId val="2081393784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2126766488"/>
+        <c:axId val="2081390728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1217,7 +1230,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126769544"/>
+        <c:crossAx val="2081393784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1225,7 +1238,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126769544"/>
+        <c:axId val="2081393784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1236,7 +1249,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126766488"/>
+        <c:crossAx val="2081390728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1283,7 +1296,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02data-ok'!$A$1</c:f>
+              <c:f>'02data-bad'!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1297,7 +1310,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'02data-ok'!$B$5:$B$8</c:f>
+              <c:f>'02data-bad'!$B$5:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1318,7 +1331,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'02data-ok'!$C$1:$C$4</c:f>
+              <c:f>'02data-bad'!$C$1:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1344,7 +1357,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02data-ok'!$A$10</c:f>
+              <c:f>'02data-bad'!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1358,7 +1371,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'02data-ok'!$B$5:$B$8</c:f>
+              <c:f>'02data-bad'!$B$5:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1379,7 +1392,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'02data-ok'!$C$9:$C$12</c:f>
+              <c:f>'02data-bad'!$C$9:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1405,7 +1418,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02data-ok'!$A$5</c:f>
+              <c:f>'02data-bad'!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1419,7 +1432,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'02data-ok'!$B$5:$B$8</c:f>
+              <c:f>'02data-bad'!$B$5:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1440,7 +1453,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'02data-ok'!$C$5:$C$8</c:f>
+              <c:f>'02data-bad'!$C$5:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1471,11 +1484,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2126800664"/>
-        <c:axId val="2126803640"/>
+        <c:axId val="2080675272"/>
+        <c:axId val="2080672280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2126800664"/>
+        <c:axId val="2080675272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1485,7 +1498,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126803640"/>
+        <c:crossAx val="2080672280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1493,7 +1506,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126803640"/>
+        <c:axId val="2080672280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1504,7 +1517,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126800664"/>
+        <c:crossAx val="2080675272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1551,7 +1564,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'03data-ok'!$A$1</c:f>
+              <c:f>'03data-beta'!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1565,7 +1578,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'03data-ok'!$B$5:$B$8</c:f>
+              <c:f>'03data-beta'!$B$5:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1586,7 +1599,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'03data-ok'!$C$1:$C$4</c:f>
+              <c:f>'03data-beta'!$C$1:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1612,7 +1625,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'03data-ok'!$A$10</c:f>
+              <c:f>'03data-beta'!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1626,7 +1639,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'03data-ok'!$B$5:$B$8</c:f>
+              <c:f>'03data-beta'!$B$5:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1647,7 +1660,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'03data-ok'!$C$9:$C$12</c:f>
+              <c:f>'03data-beta'!$C$9:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1673,7 +1686,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'03data-ok'!$A$5</c:f>
+              <c:f>'03data-beta'!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1687,7 +1700,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'03data-ok'!$B$5:$B$8</c:f>
+              <c:f>'03data-beta'!$B$5:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1708,7 +1721,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'03data-ok'!$C$5:$C$8</c:f>
+              <c:f>'03data-beta'!$C$5:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1739,11 +1752,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2140388328"/>
-        <c:axId val="2140955848"/>
+        <c:axId val="2082599560"/>
+        <c:axId val="2083695352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2140388328"/>
+        <c:axId val="2082599560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1753,7 +1766,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2140955848"/>
+        <c:crossAx val="2083695352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1761,7 +1774,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2140955848"/>
+        <c:axId val="2083695352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1772,7 +1785,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2140388328"/>
+        <c:crossAx val="2082599560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1819,7 +1832,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'04data-ok'!$A$1</c:f>
+              <c:f>'04data-beta'!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1833,7 +1846,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'04data-ok'!$B$13:$B$16</c:f>
+              <c:f>'04data-beta'!$B$13:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1854,7 +1867,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'04data-ok'!$C$1:$C$4</c:f>
+              <c:f>'04data-beta'!$C$1:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1880,7 +1893,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'04data-ok'!$A$10</c:f>
+              <c:f>'04data-beta'!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1894,7 +1907,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'04data-ok'!$B$13:$B$16</c:f>
+              <c:f>'04data-beta'!$B$13:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1915,7 +1928,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'04data-ok'!$C$9:$C$12</c:f>
+              <c:f>'04data-beta'!$C$9:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1941,7 +1954,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'04data-ok'!$A$5</c:f>
+              <c:f>'04data-beta'!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1955,7 +1968,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'04data-ok'!$B$13:$B$16</c:f>
+              <c:f>'04data-beta'!$B$13:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1976,7 +1989,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'04data-ok'!$C$5:$C$8</c:f>
+              <c:f>'04data-beta'!$C$5:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2002,7 +2015,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'04data-ok'!$A$15</c:f>
+              <c:f>'04data-beta'!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2016,7 +2029,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'04data-ok'!$B$13:$B$16</c:f>
+              <c:f>'04data-beta'!$B$13:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2037,7 +2050,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'04data-ok'!$C$13:$C$16</c:f>
+              <c:f>'04data-beta'!$C$13:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2068,11 +2081,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2126418408"/>
-        <c:axId val="-2126272568"/>
+        <c:axId val="2083927752"/>
+        <c:axId val="2083688360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2126418408"/>
+        <c:axId val="2083927752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2082,7 +2095,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126272568"/>
+        <c:crossAx val="2083688360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2090,7 +2103,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2126272568"/>
+        <c:axId val="2083688360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2101,7 +2114,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126418408"/>
+        <c:crossAx val="2083927752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2152,7 +2165,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>NotSoNaive + KingstonImproved (Distribuído)</c:v>
+                  <c:v>ZigZagOverNSNMobility</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2162,7 +2175,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'05data-running'!$B$13:$B$16</c:f>
+              <c:f>'05data-running'!$B$5:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2173,10 +2186,10 @@
                   <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2188,16 +2201,16 @@
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.15042829268292</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.83115121951219</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.3326565853658</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>26.3928780487804</c:v>
+                  <c:v>2.65182333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.20932966666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.9378753333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.2775763333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2213,7 +2226,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TSPbased (NP-hard)</c:v>
+                  <c:v>NotSoNaiveOrderedMobility</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2223,7 +2236,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'05data-running'!$B$13:$B$16</c:f>
+              <c:f>'05data-running'!$B$5:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2234,10 +2247,10 @@
                   <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2249,16 +2262,16 @@
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.615052</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.897811</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>13.823088</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>28.028619</c:v>
+                  <c:v>2.65275733333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.25548333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.7142513333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.4016293333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2274,7 +2287,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>NotSoNaive O(n2)</c:v>
+                  <c:v>NaiveOrderedMobility</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2284,7 +2297,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'05data-running'!$B$13:$B$16</c:f>
+              <c:f>'05data-running'!$B$5:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2295,10 +2308,10 @@
                   <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2310,16 +2323,16 @@
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.183175</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.293619</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.641666</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25.613135</c:v>
+                  <c:v>0.963531</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.876943</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.67018033333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.47626866666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2335,7 +2348,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Naive O(n log n)</c:v>
+                  <c:v>ZigZagOverNaiveMobility</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2345,7 +2358,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'05data-running'!$B$13:$B$16</c:f>
+              <c:f>'05data-running'!$B$5:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2356,10 +2369,10 @@
                   <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2371,16 +2384,16 @@
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.247444</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.693923</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.535141</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10.742145</c:v>
+                  <c:v>0.914449</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.84290433333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.45466766666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.77658733333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2397,11 +2410,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2139107496"/>
-        <c:axId val="2140002680"/>
+        <c:axId val="2084187336"/>
+        <c:axId val="2082577384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2139107496"/>
+        <c:axId val="2084187336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2411,7 +2424,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2140002680"/>
+        <c:crossAx val="2082577384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2419,7 +2432,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2140002680"/>
+        <c:axId val="2082577384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2430,7 +2443,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2139107496"/>
+        <c:crossAx val="2084187336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2667,15 +2680,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3981,10 +3994,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3992,267 +4005,235 @@
     <col min="1" max="1" width="34.6640625" customWidth="1"/>
     <col min="2" max="2" width="4.83203125" customWidth="1"/>
     <col min="3" max="3" width="27.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="0.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1">
         <v>2</v>
       </c>
       <c r="C1" s="4">
-        <v>3.1504282926829199</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>2.6518233333333301</v>
+      </c>
+      <c r="E1" s="7">
+        <v>42529</v>
+      </c>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>4</v>
       </c>
       <c r="C2" s="4">
-        <v>6.83115121951219</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>5.20932966666666</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="4">
-        <v>12.3326565853658</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>10.937875333333301</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4">
-        <v>26.3928780487804</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>32.2775763333333</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" s="4">
-        <v>3.1831749999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>0.96353100000000003</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6" s="4">
-        <v>6.2936189999999996</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>1.876943</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C7" s="4">
-        <v>12.641666000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>3.67018033333333</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C8" s="4">
-        <v>25.613135</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>7.4762686666666598</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" s="4">
-        <v>3.6150519999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>2.6527573333333301</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
       <c r="C10" s="4">
-        <v>6.8978109999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>5.2554833333333297</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C11" s="4">
-        <v>13.823088</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>10.7142513333333</v>
+      </c>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C12" s="4">
-        <v>28.028618999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>21.4016293333333</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
       <c r="C13" s="4">
-        <v>1.247444</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>0.91444899999999996</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B14">
         <v>4</v>
       </c>
       <c r="C14" s="4">
-        <v>2.6939229999999998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>1.8429043333333299</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C15" s="4">
-        <v>5.5351410000000003</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>3.4546676666666598</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B16">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C16" s="4">
-        <v>10.742145000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" t="s">
-        <v>32</v>
+        <v>7.77658733333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
K.IMP done and some tests to compare all of them are quite well, time to interpetrations. #macbytecodes
</commit_message>
<xml_diff>
--- a/linuxRunners/some results.xlsx
+++ b/linuxRunners/some results.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="480" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="680" yWindow="0" windowWidth="36020" windowHeight="19520" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="01data-Alpha" sheetId="2" r:id="rId1"/>
     <sheet name="02data-bad" sheetId="3" r:id="rId2"/>
     <sheet name="03data-beta" sheetId="5" r:id="rId3"/>
     <sheet name="04data-beta" sheetId="6" r:id="rId4"/>
-    <sheet name="05data-running" sheetId="7" r:id="rId5"/>
+    <sheet name="05Todos-25-erroColeta" sheetId="7" r:id="rId5"/>
+    <sheet name="05Todos-25-running" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="35">
   <si>
     <t>LOOPS=40</t>
   </si>
@@ -118,13 +119,16 @@
     <t>ZigZagOverNaiveMobility</t>
   </si>
   <si>
-    <t>POIs:  30</t>
-  </si>
-  <si>
     <t>30 é o minimo do minimo</t>
   </si>
   <si>
-    <t>Hard to run on TSP</t>
+    <t>POIs:  25</t>
+  </si>
+  <si>
+    <t>KingstonImprovedOverNaiveMobility</t>
+  </si>
+  <si>
+    <t>KingstonImprovedOverNSNMobility</t>
   </si>
 </sst>
 </file>
@@ -648,11 +652,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2081307112"/>
-        <c:axId val="2081310168"/>
+        <c:axId val="2143662152"/>
+        <c:axId val="2143665208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2081307112"/>
+        <c:axId val="2143662152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -662,7 +666,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081310168"/>
+        <c:crossAx val="2143665208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -670,7 +674,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2081310168"/>
+        <c:axId val="2143665208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -681,14 +685,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081307112"/>
+        <c:crossAx val="2143662152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -916,11 +919,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2081340200"/>
-        <c:axId val="2081343176"/>
+        <c:axId val="2143727960"/>
+        <c:axId val="2143730936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2081340200"/>
+        <c:axId val="2143727960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -930,7 +933,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081343176"/>
+        <c:crossAx val="2143730936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -938,7 +941,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2081343176"/>
+        <c:axId val="2143730936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -949,14 +952,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081340200"/>
+        <c:crossAx val="2143727960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1216,11 +1218,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2081390728"/>
-        <c:axId val="2081393784"/>
+        <c:axId val="2143778584"/>
+        <c:axId val="2143781640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2081390728"/>
+        <c:axId val="2143778584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1230,7 +1232,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081393784"/>
+        <c:crossAx val="2143781640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1238,7 +1240,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2081393784"/>
+        <c:axId val="2143781640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1249,14 +1251,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081390728"/>
+        <c:crossAx val="2143778584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1484,11 +1485,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2080675272"/>
-        <c:axId val="2080672280"/>
+        <c:axId val="2143812856"/>
+        <c:axId val="2143815832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2080675272"/>
+        <c:axId val="2143812856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1498,7 +1499,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080672280"/>
+        <c:crossAx val="2143815832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1506,7 +1507,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2080672280"/>
+        <c:axId val="2143815832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1517,14 +1518,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080675272"/>
+        <c:crossAx val="2143812856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1752,11 +1752,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2082599560"/>
-        <c:axId val="2083695352"/>
+        <c:axId val="2143855144"/>
+        <c:axId val="2143858184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2082599560"/>
+        <c:axId val="2143855144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1766,7 +1766,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083695352"/>
+        <c:crossAx val="2143858184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1774,7 +1774,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2083695352"/>
+        <c:axId val="2143858184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1785,14 +1785,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082599560"/>
+        <c:crossAx val="2143855144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2081,11 +2080,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2083927752"/>
-        <c:axId val="2083688360"/>
+        <c:axId val="2141027400"/>
+        <c:axId val="2141030584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2083927752"/>
+        <c:axId val="2141027400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2095,7 +2094,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083688360"/>
+        <c:crossAx val="2141030584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2103,7 +2102,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2083688360"/>
+        <c:axId val="2141030584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2114,14 +2113,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083927752"/>
+        <c:crossAx val="2141027400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2161,7 +2159,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'05data-running'!$A$1</c:f>
+              <c:f>'05Todos-25-erroColeta'!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2175,7 +2173,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'05data-running'!$B$5:$B$8</c:f>
+              <c:f>'05Todos-25-erroColeta'!$B$21:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2196,21 +2194,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'05data-running'!$C$1:$C$4</c:f>
+              <c:f>'05Todos-25-erroColeta'!$C$1:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.65182333333333</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.20932966666666</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10.9378753333333</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>32.2775763333333</c:v>
+                  <c:v>14.3111690434782</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.202184347826</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>79.5967245217391</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>246.752115130434</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2222,7 +2220,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'05data-running'!$A$10</c:f>
+              <c:f>'05Todos-25-erroColeta'!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2236,7 +2234,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'05data-running'!$B$5:$B$8</c:f>
+              <c:f>'05Todos-25-erroColeta'!$B$21:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2257,21 +2255,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'05data-running'!$C$9:$C$12</c:f>
+              <c:f>'05Todos-25-erroColeta'!$C$9:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.65275733333333</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.25548333333333</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10.7142513333333</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>21.4016293333333</c:v>
+                  <c:v>12.4384906896551</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.2370734482758</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49.3034048275862</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98.81574413793101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2283,7 +2281,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'05data-running'!$A$5</c:f>
+              <c:f>'05Todos-25-erroColeta'!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2297,7 +2295,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'05data-running'!$B$5:$B$8</c:f>
+              <c:f>'05Todos-25-erroColeta'!$B$21:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2318,21 +2316,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'05data-running'!$C$5:$C$8</c:f>
+              <c:f>'05Todos-25-erroColeta'!$C$5:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.963531</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.876943</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.67018033333333</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.47626866666666</c:v>
+                  <c:v>6.02996206896551</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.1768427586206</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.8780196551724</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49.4848903448275</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2344,7 +2342,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'05data-running'!$A$15</c:f>
+              <c:f>'05Todos-25-erroColeta'!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2358,7 +2356,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'05data-running'!$B$5:$B$8</c:f>
+              <c:f>'05Todos-25-erroColeta'!$B$21:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2379,21 +2377,143 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'05data-running'!$C$13:$C$16</c:f>
+              <c:f>'05Todos-25-erroColeta'!$C$13:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.914449</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.84290433333333</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.45466766666666</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.77658733333333</c:v>
+                  <c:v>7.99479929203539</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.8155982300884</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29.0805929203539</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48.5073465486725</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'05Todos-25-erroColeta'!$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KingstonImprovedOverNaiveMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'05Todos-25-erroColeta'!$B$21:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'05Todos-25-erroColeta'!$C$17:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.13002433333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.17416866666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.45380166666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.799508</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'05Todos-25-erroColeta'!$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KingstonImprovedOverNSNMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'05Todos-25-erroColeta'!$B$21:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'05Todos-25-erroColeta'!$C$21:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.40142533333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.41014033333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.6985676666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.1910646666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2410,11 +2530,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2084187336"/>
-        <c:axId val="2082577384"/>
+        <c:axId val="2141076312"/>
+        <c:axId val="2141079496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2084187336"/>
+        <c:axId val="2141076312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2424,7 +2544,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082577384"/>
+        <c:crossAx val="2141079496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2432,7 +2552,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2082577384"/>
+        <c:axId val="2141079496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2443,7 +2563,458 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2084187336"/>
+        <c:crossAx val="2141076312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'05Todos-25-running'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ZigZagOverNSNMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'05Todos-25-running'!$B$21:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'05Todos-25-running'!$C$1:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.35796166666666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.43690666666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.276859</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.4725023333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'05Todos-25-running'!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NotSoNaiveOrderedMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'05Todos-25-running'!$B$21:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'05Todos-25-running'!$C$9:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.927914</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.648262</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.77422</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.6182116666666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'05Todos-25-running'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NaiveOrderedMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'05Todos-25-running'!$B$21:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'05Todos-25-running'!$C$5:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.07737633333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.20958933333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.287052</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.09048866666666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'05Todos-25-running'!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ZigZagOverNaiveMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'05Todos-25-running'!$B$21:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'05Todos-25-running'!$C$13:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.082988</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.22913466666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.392858</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.82334366666666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'05Todos-25-running'!$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KingstonImprovedOverNaiveMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'05Todos-25-running'!$B$21:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'05Todos-25-running'!$C$17:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.069415</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.30083233333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.585063</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.608298666666659</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'05Todos-25-running'!$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KingstonImprovedOverNSNMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'05Todos-25-running'!$B$21:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'05Todos-25-running'!$C$21:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.388118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.19355566666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.9538006666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.3582083333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2145537432"/>
+        <c:axId val="2145534216"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2145537432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2145534216"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2145534216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#.##00000" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2145537432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2685,10 +3256,47 @@
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3994,10 +4602,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4018,10 +4626,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="4">
-        <v>2.6518233333333301</v>
+        <v>14.3111690434782</v>
       </c>
       <c r="E1" s="7">
-        <v>42529</v>
+        <v>42621</v>
       </c>
       <c r="G1" s="2"/>
     </row>
@@ -4033,13 +4641,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="4">
-        <v>5.20932966666666</v>
+        <v>21.202184347826002</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>28</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4050,7 +4658,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="4">
-        <v>10.937875333333301</v>
+        <v>79.596724521739105</v>
       </c>
       <c r="E3" t="s">
         <v>20</v>
@@ -4067,7 +4675,7 @@
         <v>16</v>
       </c>
       <c r="C4" s="4">
-        <v>32.2775763333333</v>
+        <v>246.75211513043399</v>
       </c>
       <c r="E4" t="s">
         <v>21</v>
@@ -4082,7 +4690,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="4">
-        <v>0.96353100000000003</v>
+        <v>6.02996206896551</v>
       </c>
       <c r="G5" s="2"/>
     </row>
@@ -4094,7 +4702,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="4">
-        <v>1.876943</v>
+        <v>12.1768427586206</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -4109,7 +4717,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="4">
-        <v>3.67018033333333</v>
+        <v>24.878019655172402</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -4124,7 +4732,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="4">
-        <v>7.4762686666666598</v>
+        <v>49.484890344827498</v>
       </c>
       <c r="G8" s="2"/>
     </row>
@@ -4136,7 +4744,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="4">
-        <v>2.6527573333333301</v>
+        <v>12.438490689655101</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
@@ -4151,7 +4759,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="4">
-        <v>5.2554833333333297</v>
+        <v>25.237073448275801</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
@@ -4166,7 +4774,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="4">
-        <v>10.7142513333333</v>
+        <v>49.303404827586199</v>
       </c>
       <c r="G11" s="2"/>
     </row>
@@ -4178,7 +4786,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="4">
-        <v>21.4016293333333</v>
+        <v>98.815744137931006</v>
       </c>
       <c r="G12" s="2"/>
     </row>
@@ -4190,14 +4798,12 @@
         <v>2</v>
       </c>
       <c r="C13" s="4">
-        <v>0.91444899999999996</v>
+        <v>7.9947992920353901</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>33</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
@@ -4207,7 +4813,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="4">
-        <v>1.8429043333333299</v>
+        <v>14.815598230088399</v>
       </c>
       <c r="E14" t="s">
         <v>17</v>
@@ -4222,7 +4828,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="4">
-        <v>3.4546676666666598</v>
+        <v>29.080592920353901</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -4233,7 +4839,437 @@
         <v>16</v>
       </c>
       <c r="C16" s="4">
-        <v>7.77658733333333</v>
+        <v>48.507346548672501</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1.13002433333333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" s="4">
+        <v>2.17416866666666</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19" s="4">
+        <v>4.45380166666666</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20">
+        <v>16</v>
+      </c>
+      <c r="C20" s="4">
+        <v>8.7995079999999994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" s="4">
+        <v>3.40142533333333</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22" s="4">
+        <v>6.41014033333333</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23" s="4">
+        <v>12.6985676666666</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24">
+        <v>16</v>
+      </c>
+      <c r="C24" s="4">
+        <v>25.191064666666598</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="34.6640625" customWidth="1"/>
+    <col min="2" max="2" width="4.83203125" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="0.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4">
+        <v>3.3579616666666601</v>
+      </c>
+      <c r="E1" s="7">
+        <v>42621</v>
+      </c>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4">
+        <v>6.4369066666666601</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4">
+        <v>13.276859</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4">
+        <v>25.472502333333299</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1.0773763333333299</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4">
+        <v>2.2095893333333301</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7" s="4">
+        <v>4.2870520000000001</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>16</v>
+      </c>
+      <c r="C8" s="4">
+        <v>9.0904886666666602</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2.9279139999999999</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" s="4">
+        <v>5.6482619999999999</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4">
+        <v>11.77422</v>
+      </c>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <v>16</v>
+      </c>
+      <c r="C12" s="4">
+        <v>22.6182116666666</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1.0829880000000001</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2.2291346666666598</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15" s="4">
+        <v>4.3928580000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>16</v>
+      </c>
+      <c r="C16" s="4">
+        <v>8.8233436666666591</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1.069415</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" s="4">
+        <v>2.30083233333333</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19" s="4">
+        <v>4.5850629999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20">
+        <v>16</v>
+      </c>
+      <c r="C20" s="4">
+        <v>9.6082986666666592</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" s="4">
+        <v>3.388118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22" s="4">
+        <v>6.1935556666666596</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23" s="4">
+        <v>11.9538006666666</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24">
+        <v>16</v>
+      </c>
+      <c r="C24" s="4">
+        <v>25.358208333333302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Setting more evaluations to lac server. #macbytecodes
</commit_message>
<xml_diff>
--- a/linuxRunners/some results.xlsx
+++ b/linuxRunners/some results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="0" windowWidth="27220" windowHeight="19620" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="680" yWindow="0" windowWidth="33440" windowHeight="19540" tabRatio="757" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="01data-Alpha" sheetId="2" r:id="rId1"/>
@@ -12,7 +12,8 @@
     <sheet name="03data-beta" sheetId="5" r:id="rId3"/>
     <sheet name="04data-beta" sheetId="6" r:id="rId4"/>
     <sheet name="05Todos-25-erroColeta" sheetId="7" r:id="rId5"/>
-    <sheet name="05Todos-25-running" sheetId="8" r:id="rId6"/>
+    <sheet name="05Todos-25-duvida" sheetId="8" r:id="rId6"/>
+    <sheet name="06-20-running" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="47">
   <si>
     <t>LOOPS=40</t>
   </si>
@@ -130,6 +131,42 @@
   <si>
     <t>KingstonImprovedOverNSNMobility</t>
   </si>
+  <si>
+    <t>Só 10 rodadas ao inves de 30 e limite de 900 segundos</t>
+  </si>
+  <si>
+    <t>ACHO QUE DEU ERRO NO TSP</t>
+  </si>
+  <si>
+    <t>MAQUINA</t>
+  </si>
+  <si>
+    <t>MISTURADA</t>
+  </si>
+  <si>
+    <t>mandei rodar 10 depois rodo mais 20</t>
+  </si>
+  <si>
+    <t>ROUNDS=7500000</t>
+  </si>
+  <si>
+    <t>REFRESHRATE=7500000</t>
+  </si>
+  <si>
+    <t>dobrei</t>
+  </si>
+  <si>
+    <t>simplifiquei</t>
+  </si>
+  <si>
+    <t>tudo no LAC</t>
+  </si>
+  <si>
+    <t>diminui</t>
+  </si>
+  <si>
+    <t>LOOPS=5</t>
+  </si>
 </sst>
 </file>
 
@@ -139,7 +176,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -168,6 +205,44 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="36"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -277,7 +352,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -286,6 +361,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="87">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -716,11 +798,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2124981864"/>
-        <c:axId val="-2124978760"/>
+        <c:axId val="2134140200"/>
+        <c:axId val="2134137128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2124981864"/>
+        <c:axId val="2134140200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -730,7 +812,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124978760"/>
+        <c:crossAx val="2134137128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -738,7 +820,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2124978760"/>
+        <c:axId val="2134137128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -749,7 +831,970 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124981864"/>
+        <c:crossAx val="2134140200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'06-20-running'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ZigZagOverNSNMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'06-20-running'!$C$1:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.35796166666666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.43690666666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.276859</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.4725023333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'06-20-running'!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NotSoNaiveOrderedMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'06-20-running'!$C$9:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.927914</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.648262</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.77422</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.6182116666666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'06-20-running'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NaiveOrderedMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'06-20-running'!$C$5:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.07737633333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.20958933333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.287052</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.09048866666666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'06-20-running'!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ZigZagOverNaiveMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'06-20-running'!$C$13:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.082988</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.22913466666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.392858</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.82334366666666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'06-20-running'!$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KingstonImprovedOverNaiveMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'06-20-running'!$C$17:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.069415</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.30083233333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.585063</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.608298666666659</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'06-20-running'!$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KingstonImprovedOverNSNMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'06-20-running'!$C$21:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.388118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.19355566666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.9538006666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.3582083333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'06-20-running'!$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TSPbasedMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'06-20-running'!$C$25:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.24429533333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.506488</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.4277993333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.1466703333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'06-20-running'!$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AntiTSPbasedMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'06-20-running'!$C$29:$C$32</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.897711</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.053749</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.271979</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.771024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2129817928"/>
+        <c:axId val="2129978424"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2129817928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2129978424"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2129978424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#.##00000" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2129817928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'06-20-running'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ZigZagOverNSNMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'06-20-running'!$C$1:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.35796166666666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.43690666666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.276859</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.4725023333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'06-20-running'!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NotSoNaiveOrderedMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'06-20-running'!$C$9:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.927914</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.648262</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.77422</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.6182116666666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'06-20-running'!$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KingstonImprovedOverNSNMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'06-20-running'!$C$21:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.388118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.19355566666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.9538006666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.3582083333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'06-20-running'!$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TSPbasedMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'06-20-running'!$C$25:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.24429533333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.506488</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.4277993333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.1466703333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'06-20-running'!$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AntiTSPbasedMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'06-20-running'!$C$29:$C$32</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.897711</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.053749</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.271979</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.771024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2143190152"/>
+        <c:axId val="2143122968"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2143190152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2143122968"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2143122968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#.##00000" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2143190152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -983,11 +2028,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2124902104"/>
-        <c:axId val="-2124899128"/>
+        <c:axId val="2134074392"/>
+        <c:axId val="2134071400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2124902104"/>
+        <c:axId val="2134074392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -997,7 +2042,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124899128"/>
+        <c:crossAx val="2134071400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1005,7 +2050,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2124899128"/>
+        <c:axId val="2134071400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1016,13 +2061,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124902104"/>
+        <c:crossAx val="2134074392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1282,11 +2328,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2124848008"/>
-        <c:axId val="-2124844952"/>
+        <c:axId val="2134023928"/>
+        <c:axId val="2134020856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2124848008"/>
+        <c:axId val="2134023928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1296,7 +2342,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124844952"/>
+        <c:crossAx val="2134020856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1304,7 +2350,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2124844952"/>
+        <c:axId val="2134020856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1315,13 +2361,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124848008"/>
+        <c:crossAx val="2134023928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1549,11 +2596,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2124814072"/>
-        <c:axId val="-2124811096"/>
+        <c:axId val="2133989992"/>
+        <c:axId val="2133987000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2124814072"/>
+        <c:axId val="2133989992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1563,7 +2610,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124811096"/>
+        <c:crossAx val="2133987000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1571,7 +2618,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2124811096"/>
+        <c:axId val="2133987000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1582,13 +2629,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124814072"/>
+        <c:crossAx val="2133989992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1816,11 +2864,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2124771448"/>
-        <c:axId val="-2124768408"/>
+        <c:axId val="2133947368"/>
+        <c:axId val="2133944312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2124771448"/>
+        <c:axId val="2133947368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1830,7 +2878,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124768408"/>
+        <c:crossAx val="2133944312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1838,7 +2886,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2124768408"/>
+        <c:axId val="2133944312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1849,13 +2897,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124771448"/>
+        <c:crossAx val="2133947368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2144,11 +3193,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2124723400"/>
-        <c:axId val="-2124720216"/>
+        <c:axId val="2133899320"/>
+        <c:axId val="2133896120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2124723400"/>
+        <c:axId val="2133899320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2158,7 +3207,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124720216"/>
+        <c:crossAx val="2133896120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2166,7 +3215,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2124720216"/>
+        <c:axId val="2133896120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2177,13 +3226,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124723400"/>
+        <c:crossAx val="2133899320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2594,11 +3644,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2124665240"/>
-        <c:axId val="-2124662040"/>
+        <c:axId val="2135232408"/>
+        <c:axId val="2135235608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2124665240"/>
+        <c:axId val="2135232408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2608,7 +3658,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124662040"/>
+        <c:crossAx val="2135235608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2616,7 +3666,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2124662040"/>
+        <c:axId val="2135235608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2627,13 +3677,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124665240"/>
+        <c:crossAx val="2135232408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2673,7 +3724,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'05Todos-25-running'!$A$1</c:f>
+              <c:f>'05Todos-25-duvida'!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2687,7 +3738,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'05Todos-25-running'!$B$21:$B$24</c:f>
+              <c:f>'05Todos-25-duvida'!$B$29:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2708,7 +3759,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'05Todos-25-running'!$C$1:$C$4</c:f>
+              <c:f>'05Todos-25-duvida'!$C$1:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2734,7 +3785,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'05Todos-25-running'!$A$10</c:f>
+              <c:f>'05Todos-25-duvida'!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2748,7 +3799,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'05Todos-25-running'!$B$21:$B$24</c:f>
+              <c:f>'05Todos-25-duvida'!$B$29:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2769,7 +3820,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'05Todos-25-running'!$C$9:$C$12</c:f>
+              <c:f>'05Todos-25-duvida'!$C$9:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2795,7 +3846,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'05Todos-25-running'!$A$5</c:f>
+              <c:f>'05Todos-25-duvida'!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2809,7 +3860,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'05Todos-25-running'!$B$21:$B$24</c:f>
+              <c:f>'05Todos-25-duvida'!$B$29:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2830,7 +3881,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'05Todos-25-running'!$C$5:$C$8</c:f>
+              <c:f>'05Todos-25-duvida'!$C$5:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2856,7 +3907,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'05Todos-25-running'!$A$15</c:f>
+              <c:f>'05Todos-25-duvida'!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2870,7 +3921,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'05Todos-25-running'!$B$21:$B$24</c:f>
+              <c:f>'05Todos-25-duvida'!$B$29:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2891,7 +3942,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'05Todos-25-running'!$C$13:$C$16</c:f>
+              <c:f>'05Todos-25-duvida'!$C$13:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2917,7 +3968,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'05Todos-25-running'!$A$17</c:f>
+              <c:f>'05Todos-25-duvida'!$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2931,7 +3982,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'05Todos-25-running'!$B$21:$B$24</c:f>
+              <c:f>'05Todos-25-duvida'!$B$29:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2952,7 +4003,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'05Todos-25-running'!$C$17:$C$20</c:f>
+              <c:f>'05Todos-25-duvida'!$C$17:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2978,7 +4029,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'05Todos-25-running'!$A$21</c:f>
+              <c:f>'05Todos-25-duvida'!$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2992,7 +4043,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'05Todos-25-running'!$B$21:$B$24</c:f>
+              <c:f>'05Todos-25-duvida'!$B$29:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3013,7 +4064,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'05Todos-25-running'!$C$21:$C$24</c:f>
+              <c:f>'05Todos-25-duvida'!$C$21:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3028,6 +4079,128 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>25.3582083333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'05Todos-25-duvida'!$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TSPbasedMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'05Todos-25-duvida'!$B$29:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'05Todos-25-duvida'!$C$25:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.24429533333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.506488</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.4277993333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.1466703333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'05Todos-25-duvida'!$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AntiTSPbasedMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'05Todos-25-duvida'!$B$29:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'05Todos-25-duvida'!$C$29:$C$32</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.897711</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.053749</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.271979</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.771024</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3044,11 +4217,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2126331464"/>
-        <c:axId val="-2126328264"/>
+        <c:axId val="2135287176"/>
+        <c:axId val="2135290376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2126331464"/>
+        <c:axId val="2135287176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3058,7 +4231,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126328264"/>
+        <c:crossAx val="2135290376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3066,7 +4239,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2126328264"/>
+        <c:axId val="2135290376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3077,7 +4250,397 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126331464"/>
+        <c:crossAx val="2135287176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'05Todos-25-duvida'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ZigZagOverNSNMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'05Todos-25-duvida'!$B$29:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'05Todos-25-duvida'!$C$1:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.35796166666666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.43690666666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.276859</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.4725023333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'05Todos-25-duvida'!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NotSoNaiveOrderedMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'05Todos-25-duvida'!$B$29:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'05Todos-25-duvida'!$C$9:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.927914</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.648262</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.77422</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.6182116666666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'05Todos-25-duvida'!$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KingstonImprovedOverNSNMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'05Todos-25-duvida'!$B$29:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'05Todos-25-duvida'!$C$21:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.388118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.19355566666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.9538006666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.3582083333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'05Todos-25-duvida'!$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TSPbasedMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'05Todos-25-duvida'!$B$29:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'05Todos-25-duvida'!$C$25:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.24429533333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.506488</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.4277993333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.1466703333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'05Todos-25-duvida'!$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AntiTSPbasedMobility</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'05Todos-25-duvida'!$B$29:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'05Todos-25-duvida'!$C$29:$C$32</c:f>
+              <c:numCache>
+                <c:formatCode>#.##00000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.897711</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.053749</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.271979</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.771024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2139378744"/>
+        <c:axId val="2139381752"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2139378744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2139381752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2139381752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#.##00000" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2139378744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3351,15 +4914,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
+      <xdr:colOff>25399</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>406399</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>118533</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3375,6 +4938,107 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>25399</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>406399</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>118533</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4667,7 +6331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="C17" sqref="C17:C24"/>
     </sheetView>
   </sheetViews>
@@ -5007,10 +6671,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C16"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5097,7 +6761,12 @@
       <c r="C5" s="4">
         <v>1.0773763333333299</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
@@ -5334,6 +7003,567 @@
       <c r="C24" s="4">
         <v>25.358208333333302</v>
       </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="5">
+        <v>2</v>
+      </c>
+      <c r="C25" s="8">
+        <v>3.24429533333333</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="5">
+        <v>4</v>
+      </c>
+      <c r="C26" s="8">
+        <v>6.506488</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="5">
+        <v>8</v>
+      </c>
+      <c r="C27" s="8">
+        <v>13.427799333333301</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="5">
+        <v>16</v>
+      </c>
+      <c r="C28" s="8">
+        <v>26.146670333333301</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="5">
+        <v>2</v>
+      </c>
+      <c r="C29" s="8">
+        <v>0.89771100000000004</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="5">
+        <v>4</v>
+      </c>
+      <c r="C30" s="8">
+        <v>1.053749</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="5">
+        <v>8</v>
+      </c>
+      <c r="C31" s="8">
+        <v>1.271979</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="5">
+        <v>16</v>
+      </c>
+      <c r="C32" s="8">
+        <v>1.7710239999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="36">
+      <c r="A39" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="34.6640625" customWidth="1"/>
+    <col min="2" max="2" width="4.83203125" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="0.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1" s="8">
+        <v>3.3579616666666601</v>
+      </c>
+      <c r="E1" s="7">
+        <v>42621</v>
+      </c>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2" s="8">
+        <v>6.4369066666666601</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3" s="8">
+        <v>13.276859</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4">
+        <v>16</v>
+      </c>
+      <c r="C4" s="8">
+        <v>25.472502333333299</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1.0773763333333299</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="45">
+      <c r="A6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="11">
+        <v>4</v>
+      </c>
+      <c r="C6" s="8">
+        <v>2.2095893333333301</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="I6" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="11">
+        <v>8</v>
+      </c>
+      <c r="C7" s="8">
+        <v>4.2870520000000001</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11">
+        <v>16</v>
+      </c>
+      <c r="C8" s="8">
+        <v>9.0904886666666602</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="11">
+        <v>2</v>
+      </c>
+      <c r="C9" s="8">
+        <v>2.9279139999999999</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="11">
+        <v>4</v>
+      </c>
+      <c r="C10" s="8">
+        <v>5.6482619999999999</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="11">
+        <v>8</v>
+      </c>
+      <c r="C11" s="8">
+        <v>11.77422</v>
+      </c>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="11">
+        <v>16</v>
+      </c>
+      <c r="C12" s="8">
+        <v>22.6182116666666</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="11">
+        <v>2</v>
+      </c>
+      <c r="C13" s="8">
+        <v>1.0829880000000001</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="11">
+        <v>4</v>
+      </c>
+      <c r="C14" s="8">
+        <v>2.2291346666666598</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="11">
+        <v>8</v>
+      </c>
+      <c r="C15" s="8">
+        <v>4.3928580000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="11">
+        <v>16</v>
+      </c>
+      <c r="C16" s="8">
+        <v>8.8233436666666591</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="11">
+        <v>2</v>
+      </c>
+      <c r="C17" s="8">
+        <v>1.069415</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="11">
+        <v>4</v>
+      </c>
+      <c r="C18" s="8">
+        <v>2.30083233333333</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="11">
+        <v>8</v>
+      </c>
+      <c r="C19" s="8">
+        <v>4.5850629999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="11">
+        <v>16</v>
+      </c>
+      <c r="C20" s="8">
+        <v>9.6082986666666592</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="11">
+        <v>2</v>
+      </c>
+      <c r="C21" s="8">
+        <v>3.388118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="11">
+        <v>4</v>
+      </c>
+      <c r="C22" s="8">
+        <v>6.1935556666666596</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="11">
+        <v>8</v>
+      </c>
+      <c r="C23" s="8">
+        <v>11.9538006666666</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="11">
+        <v>16</v>
+      </c>
+      <c r="C24" s="8">
+        <v>25.358208333333302</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="11">
+        <v>2</v>
+      </c>
+      <c r="C25" s="8">
+        <v>3.24429533333333</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="11">
+        <v>4</v>
+      </c>
+      <c r="C26" s="8">
+        <v>6.506488</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="11">
+        <v>8</v>
+      </c>
+      <c r="C27" s="8">
+        <v>13.427799333333301</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="11">
+        <v>16</v>
+      </c>
+      <c r="C28" s="8">
+        <v>26.146670333333301</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="11">
+        <v>2</v>
+      </c>
+      <c r="C29" s="8">
+        <v>0.89771100000000004</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="11">
+        <v>4</v>
+      </c>
+      <c r="C30" s="8">
+        <v>1.053749</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="11">
+        <v>8</v>
+      </c>
+      <c r="C31" s="8">
+        <v>1.271979</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="11">
+        <v>16</v>
+      </c>
+      <c r="C32" s="8">
+        <v>1.7710239999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="6"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="12"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="6"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="6"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="6"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="C37" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Just a backup to sync machines. #macbytecodes
</commit_message>
<xml_diff>
--- a/linuxRunners/some results.xlsx
+++ b/linuxRunners/some results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="0" windowWidth="33440" windowHeight="19540" tabRatio="757" activeTab="6"/>
+    <workbookView xWindow="680" yWindow="0" windowWidth="30900" windowHeight="18960" tabRatio="757" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="01data-Alpha" sheetId="2" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="04data-beta" sheetId="6" r:id="rId4"/>
     <sheet name="05Todos-25-erroColeta" sheetId="7" r:id="rId5"/>
     <sheet name="05Todos-25-duvida" sheetId="8" r:id="rId6"/>
-    <sheet name="06-20-running" sheetId="9" r:id="rId7"/>
+    <sheet name="06-20-PARTIAL-running" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -144,9 +144,6 @@
     <t>MISTURADA</t>
   </si>
   <si>
-    <t>mandei rodar 10 depois rodo mais 20</t>
-  </si>
-  <si>
     <t>ROUNDS=7500000</t>
   </si>
   <si>
@@ -162,10 +159,13 @@
     <t>tudo no LAC</t>
   </si>
   <si>
-    <t>diminui</t>
+    <t>LOOPS=5</t>
   </si>
   <si>
-    <t>LOOPS=5</t>
+    <t>mandei rodar 5 depois rodo mais 25</t>
+  </si>
+  <si>
+    <t>diminui MUITO, quando mais pontos, melhor vai ficando o TSP</t>
   </si>
 </sst>
 </file>
@@ -878,7 +878,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'06-20-running'!$A$1</c:f>
+              <c:f>'06-20-PARTIAL-running'!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -892,7 +892,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:f>'06-20-PARTIAL-running'!$B$29:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -913,21 +913,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'06-20-running'!$C$1:$C$4</c:f>
+              <c:f>'06-20-PARTIAL-running'!$C$1:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.35796166666666</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.43690666666666</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>13.276859</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25.4725023333333</c:v>
+                  <c:v>3.56006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.06631</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.47832</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.605262</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -939,7 +939,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'06-20-running'!$A$10</c:f>
+              <c:f>'06-20-PARTIAL-running'!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -953,7 +953,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:f>'06-20-PARTIAL-running'!$B$29:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -974,21 +974,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'06-20-running'!$C$9:$C$12</c:f>
+              <c:f>'06-20-PARTIAL-running'!$C$9:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.927914</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.648262</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11.77422</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>22.6182116666666</c:v>
+                  <c:v>3.055038</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.820196</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.254448</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.781112</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1000,7 +1000,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'06-20-running'!$A$5</c:f>
+              <c:f>'06-20-PARTIAL-running'!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1014,7 +1014,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:f>'06-20-PARTIAL-running'!$B$29:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1035,21 +1035,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'06-20-running'!$C$5:$C$8</c:f>
+              <c:f>'06-20-PARTIAL-running'!$C$5:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.07737633333333</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.20958933333333</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.287052</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.09048866666666</c:v>
+                  <c:v>1.43876333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.634895</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.57842333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.4733733333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1061,7 +1061,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'06-20-running'!$A$15</c:f>
+              <c:f>'06-20-PARTIAL-running'!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1075,7 +1075,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:f>'06-20-PARTIAL-running'!$B$29:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1096,21 +1096,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'06-20-running'!$C$13:$C$16</c:f>
+              <c:f>'06-20-PARTIAL-running'!$C$13:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.082988</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.22913466666666</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.392858</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.82334366666666</c:v>
+                  <c:v>1.411228</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.497232</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.370154</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.809774</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1122,7 +1122,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'06-20-running'!$A$17</c:f>
+              <c:f>'06-20-PARTIAL-running'!$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1136,7 +1136,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:f>'06-20-PARTIAL-running'!$B$29:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1157,21 +1157,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'06-20-running'!$C$17:$C$20</c:f>
+              <c:f>'06-20-PARTIAL-running'!$C$17:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.069415</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.30083233333333</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.585063</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.608298666666659</c:v>
+                  <c:v>1.316112</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.763438</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.909356</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.105646</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1183,7 +1183,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'06-20-running'!$A$21</c:f>
+              <c:f>'06-20-PARTIAL-running'!$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1197,7 +1197,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:f>'06-20-PARTIAL-running'!$B$29:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1218,21 +1218,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'06-20-running'!$C$21:$C$24</c:f>
+              <c:f>'06-20-PARTIAL-running'!$C$21:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.388118</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.19355566666666</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11.9538006666666</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25.3582083333333</c:v>
+                  <c:v>4.103518</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.234336000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.4305</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.378204</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1244,7 +1244,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'06-20-running'!$A$26</c:f>
+              <c:f>'06-20-PARTIAL-running'!$A$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1258,7 +1258,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:f>'06-20-PARTIAL-running'!$B$29:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1279,21 +1279,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'06-20-running'!$C$25:$C$28</c:f>
+              <c:f>'06-20-PARTIAL-running'!$C$25:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.24429533333333</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.506488</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>13.4277993333333</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>26.1466703333333</c:v>
+                  <c:v>4.58248181818181</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.79682909090909</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.82944</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.201949090909</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1305,7 +1305,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>'06-20-running'!$A$30</c:f>
+              <c:f>'06-20-PARTIAL-running'!$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1319,7 +1319,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:f>'06-20-PARTIAL-running'!$B$29:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1340,7 +1340,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'06-20-running'!$C$29:$C$32</c:f>
+              <c:f>'06-20-PARTIAL-running'!$C$29:$C$32</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1451,7 +1451,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'06-20-running'!$A$1</c:f>
+              <c:f>'06-20-PARTIAL-running'!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1465,7 +1465,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:f>'06-20-PARTIAL-running'!$B$29:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1486,21 +1486,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'06-20-running'!$C$1:$C$4</c:f>
+              <c:f>'06-20-PARTIAL-running'!$C$1:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.35796166666666</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.43690666666666</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>13.276859</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25.4725023333333</c:v>
+                  <c:v>3.56006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.06631</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.47832</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.605262</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1512,7 +1512,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'06-20-running'!$A$10</c:f>
+              <c:f>'06-20-PARTIAL-running'!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1526,7 +1526,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:f>'06-20-PARTIAL-running'!$B$29:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1547,21 +1547,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'06-20-running'!$C$9:$C$12</c:f>
+              <c:f>'06-20-PARTIAL-running'!$C$9:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.927914</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.648262</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11.77422</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>22.6182116666666</c:v>
+                  <c:v>3.055038</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.820196</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.254448</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.781112</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1573,7 +1573,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'06-20-running'!$A$21</c:f>
+              <c:f>'06-20-PARTIAL-running'!$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1587,7 +1587,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:f>'06-20-PARTIAL-running'!$B$29:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1608,21 +1608,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'06-20-running'!$C$21:$C$24</c:f>
+              <c:f>'06-20-PARTIAL-running'!$C$21:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.388118</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.19355566666666</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11.9538006666666</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25.3582083333333</c:v>
+                  <c:v>4.103518</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.234336000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.4305</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.378204</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1634,7 +1634,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'06-20-running'!$A$26</c:f>
+              <c:f>'06-20-PARTIAL-running'!$A$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1648,7 +1648,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:f>'06-20-PARTIAL-running'!$B$29:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1669,21 +1669,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'06-20-running'!$C$25:$C$28</c:f>
+              <c:f>'06-20-PARTIAL-running'!$C$25:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.24429533333333</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.506488</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>13.4277993333333</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>26.1466703333333</c:v>
+                  <c:v>4.58248181818181</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.79682909090909</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.82944</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.201949090909</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1695,7 +1695,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'06-20-running'!$A$30</c:f>
+              <c:f>'06-20-PARTIAL-running'!$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1709,7 +1709,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'06-20-running'!$B$29:$B$32</c:f>
+              <c:f>'06-20-PARTIAL-running'!$B$29:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1730,7 +1730,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'06-20-running'!$C$29:$C$32</c:f>
+              <c:f>'06-20-PARTIAL-running'!$C$29:$C$32</c:f>
               <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1801,6 +1801,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6331,7 +6332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17:C24"/>
     </sheetView>
   </sheetViews>
@@ -6674,7 +6675,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="Z116" sqref="Z116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7119,7 +7120,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7140,7 +7141,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="8">
-        <v>3.3579616666666601</v>
+        <v>3.56006</v>
       </c>
       <c r="E1" s="7">
         <v>42621</v>
@@ -7155,13 +7156,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="8">
-        <v>6.4369066666666601</v>
+        <v>7.0663099999999996</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -7172,13 +7173,13 @@
         <v>8</v>
       </c>
       <c r="C3" s="8">
-        <v>13.276859</v>
+        <v>13.47832</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -7189,10 +7190,10 @@
         <v>16</v>
       </c>
       <c r="C4" s="8">
-        <v>25.472502333333299</v>
+        <v>27.605262</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G4" s="2"/>
     </row>
@@ -7204,13 +7205,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="8">
-        <v>1.0773763333333299</v>
+        <v>1.4387633333333301</v>
       </c>
       <c r="E5" t="s">
         <v>37</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="45">
@@ -7221,14 +7222,14 @@
         <v>4</v>
       </c>
       <c r="C6" s="8">
-        <v>2.2095893333333301</v>
+        <v>2.6348950000000002</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="2"/>
       <c r="I6" s="13" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -7239,7 +7240,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="8">
-        <v>4.2870520000000001</v>
+        <v>5.5784233333333297</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -7254,7 +7255,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="8">
-        <v>9.0904886666666602</v>
+        <v>11.473373333333299</v>
       </c>
       <c r="G8" s="2"/>
     </row>
@@ -7266,7 +7267,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="8">
-        <v>2.9279139999999999</v>
+        <v>3.0550380000000001</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
@@ -7281,7 +7282,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="8">
-        <v>5.6482619999999999</v>
+        <v>6.8201960000000001</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
@@ -7296,7 +7297,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="8">
-        <v>11.77422</v>
+        <v>12.254448</v>
       </c>
       <c r="G11" s="2"/>
     </row>
@@ -7308,7 +7309,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="8">
-        <v>22.6182116666666</v>
+        <v>24.781112</v>
       </c>
       <c r="G12" s="2"/>
     </row>
@@ -7320,13 +7321,13 @@
         <v>2</v>
       </c>
       <c r="C13" s="8">
-        <v>1.0829880000000001</v>
+        <v>1.4112279999999999</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>18</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -7337,7 +7338,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="8">
-        <v>2.2291346666666598</v>
+        <v>2.4972319999999999</v>
       </c>
       <c r="E14" t="s">
         <v>17</v>
@@ -7352,7 +7353,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="8">
-        <v>4.3928580000000004</v>
+        <v>5.3701540000000003</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -7363,7 +7364,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="8">
-        <v>8.8233436666666591</v>
+        <v>10.809774000000001</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -7374,7 +7375,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="8">
-        <v>1.069415</v>
+        <v>1.3161119999999999</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -7385,7 +7386,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="8">
-        <v>2.30083233333333</v>
+        <v>2.7634379999999998</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -7396,7 +7397,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="8">
-        <v>4.5850629999999999</v>
+        <v>5.9093559999999998</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -7407,7 +7408,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="8">
-        <v>9.6082986666666592</v>
+        <v>11.105646</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -7418,7 +7419,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="8">
-        <v>3.388118</v>
+        <v>4.1035180000000002</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -7429,7 +7430,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="8">
-        <v>6.1935556666666596</v>
+        <v>8.2343360000000008</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -7440,7 +7441,7 @@
         <v>8</v>
       </c>
       <c r="C23" s="8">
-        <v>11.9538006666666</v>
+        <v>15.4305</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -7451,7 +7452,7 @@
         <v>16</v>
       </c>
       <c r="C24" s="8">
-        <v>25.358208333333302</v>
+        <v>32.378203999999997</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -7462,7 +7463,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="8">
-        <v>3.24429533333333</v>
+        <v>4.5824818181818099</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -7473,7 +7474,7 @@
         <v>4</v>
       </c>
       <c r="C26" s="8">
-        <v>6.506488</v>
+        <v>6.7968290909090898</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -7484,7 +7485,7 @@
         <v>8</v>
       </c>
       <c r="C27" s="8">
-        <v>13.427799333333301</v>
+        <v>12.82944</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -7495,7 +7496,7 @@
         <v>16</v>
       </c>
       <c r="C28" s="8">
-        <v>26.146670333333301</v>
+        <v>24.201949090909</v>
       </c>
     </row>
     <row r="29" spans="1:3">

</xml_diff>